<commit_message>
write DMI to excel. modify basic_DMI.xlsx
</commit_message>
<xml_diff>
--- a/basic bk/basic_DMI.xlsx
+++ b/basic bk/basic_DMI.xlsx
@@ -1,88 +1,89 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28615"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding4Fun\Python\twStockAnalysis\CompanyData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mussina/Documents/GitRepo/Self/TwStockAnalysis/basic bk/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="24000" windowHeight="13540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>日期</t>
   </si>
   <si>
+    <t>最高價</t>
+  </si>
+  <si>
+    <t>最低價</t>
+  </si>
+  <si>
     <t>收盤價</t>
   </si>
   <si>
-    <t>最高價</t>
-  </si>
-  <si>
-    <t>最低價</t>
-  </si>
-  <si>
     <t>+DM</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>-DM</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>+DM'</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>-DM'</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Ht - Lt</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Ht - Ct-1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Lt - Ct-1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>TR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>+ADM</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>-ADM</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>ATR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>+DI</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>-DI</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DXt</t>
+  </si>
+  <si>
+    <t>ADXt</t>
   </si>
   <si>
     <t>DMO(Directional Movement Oscillator)</t>
@@ -92,11 +93,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -104,15 +105,8 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="新細明體"/>
-      <family val="3"/>
-      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -151,15 +145,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -167,15 +160,12 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -220,9 +210,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -255,9 +245,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -464,26 +454,26 @@
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="18" max="18" width="44.75" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="31.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -527,12 +517,14 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>